<commit_message>
bf: add tas1 forms
</commit_message>
<xml_diff>
--- a/LF/TAS/Burkina Faso/2024/jan/bf_lf_tas1_202401_1_site.xlsx
+++ b/LF/TAS/Burkina Faso/2024/jan/bf_lf_tas1_202401_1_site.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\LF\TAS\Burkina Faso\2024\jan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bonhe\Repositories\dsa-forms\LF\TAS\Burkina Faso\2024\jan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E335BC53-E53D-4E17-A145-38E68557DBFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEF81974-AF79-4BA0-8FD2-156811D1E5B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="126">
   <si>
     <t>form_title</t>
   </si>
@@ -116,18 +116,6 @@
     <t>select_one operateur_list</t>
   </si>
   <si>
-    <t>01</t>
-  </si>
-  <si>
-    <t>02</t>
-  </si>
-  <si>
-    <t>03</t>
-  </si>
-  <si>
-    <t>04</t>
-  </si>
-  <si>
     <t>default_language</t>
   </si>
   <si>
@@ -248,12 +236,6 @@
     <t>csps_list = ${c_nom_CSPS}</t>
   </si>
   <si>
-    <t>05</t>
-  </si>
-  <si>
-    <t>06</t>
-  </si>
-  <si>
     <t>survey_type</t>
   </si>
   <si>
@@ -399,6 +381,42 @@
   </si>
   <si>
     <t xml:space="preserve">La valeur saisie doit être en décimal à 2 chiffres après la virgule </t>
+  </si>
+  <si>
+    <t>EN01</t>
+  </si>
+  <si>
+    <t>EN02</t>
+  </si>
+  <si>
+    <t>EN03</t>
+  </si>
+  <si>
+    <t>EN04</t>
+  </si>
+  <si>
+    <t>EN05</t>
+  </si>
+  <si>
+    <t>EN06</t>
+  </si>
+  <si>
+    <t>EN07</t>
+  </si>
+  <si>
+    <t>EN08</t>
+  </si>
+  <si>
+    <t>EN09</t>
+  </si>
+  <si>
+    <t>EN10</t>
+  </si>
+  <si>
+    <t>EN11</t>
+  </si>
+  <si>
+    <t>EN12</t>
   </si>
 </sst>
 </file>
@@ -549,7 +567,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -592,8 +610,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -933,13 +950,13 @@
         <v>10</v>
       </c>
       <c r="K1" s="12" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="L1" s="12" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="M1" s="12" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -947,7 +964,7 @@
         <v>24</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>11</v>
@@ -964,16 +981,16 @@
     </row>
     <row r="3" spans="1:13" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
@@ -985,13 +1002,13 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -1004,13 +1021,13 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
@@ -1021,18 +1038,18 @@
         <v>12</v>
       </c>
       <c r="J5" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
@@ -1043,18 +1060,18 @@
         <v>12</v>
       </c>
       <c r="J6" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
@@ -1065,26 +1082,26 @@
         <v>12</v>
       </c>
       <c r="J7" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
       <c r="F8" s="6" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="H8" s="6"/>
       <c r="I8" s="6" t="s">
@@ -1093,16 +1110,16 @@
     </row>
     <row r="9" spans="1:13" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
@@ -1128,13 +1145,13 @@
         <v>13</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>14</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
@@ -1150,7 +1167,7 @@
         <v>15</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>16</v>
@@ -1168,7 +1185,7 @@
         <v>22</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -1176,7 +1193,7 @@
         <v>17</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
@@ -1194,11 +1211,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G58"/>
+  <dimension ref="A1:G64"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G49" sqref="G49:G58"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1225,24 +1242,24 @@
         <v>20</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>25</v>
+      <c r="B2" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>114</v>
       </c>
       <c r="D2" s="9"/>
     </row>
@@ -1250,11 +1267,11 @@
       <c r="A3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" s="14" t="s">
-        <v>26</v>
+      <c r="B3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C3" t="s">
+        <v>115</v>
       </c>
       <c r="D3" s="9"/>
     </row>
@@ -1262,11 +1279,11 @@
       <c r="A4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" s="14" t="s">
-        <v>27</v>
+      <c r="B4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C4" t="s">
+        <v>116</v>
       </c>
       <c r="D4" s="9"/>
     </row>
@@ -1274,11 +1291,11 @@
       <c r="A5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>28</v>
+      <c r="B5" t="s">
+        <v>117</v>
+      </c>
+      <c r="C5" t="s">
+        <v>117</v>
       </c>
       <c r="D5" s="9"/>
     </row>
@@ -1286,11 +1303,11 @@
       <c r="A6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>69</v>
+      <c r="B6" t="s">
+        <v>118</v>
+      </c>
+      <c r="C6" t="s">
+        <v>118</v>
       </c>
       <c r="D6" s="9"/>
     </row>
@@ -1298,634 +1315,703 @@
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>70</v>
+      <c r="B7" t="s">
+        <v>119</v>
+      </c>
+      <c r="C7" t="s">
+        <v>119</v>
       </c>
       <c r="D7" s="9"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="10"/>
+      <c r="A8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" t="s">
+        <v>120</v>
+      </c>
+      <c r="C8" t="s">
+        <v>120</v>
+      </c>
+      <c r="D8" s="9"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D9" s="10"/>
+        <v>23</v>
+      </c>
+      <c r="B9" t="s">
+        <v>121</v>
+      </c>
+      <c r="C9" t="s">
+        <v>121</v>
+      </c>
+      <c r="D9" s="9"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D10" s="10"/>
+        <v>23</v>
+      </c>
+      <c r="B10" t="s">
+        <v>122</v>
+      </c>
+      <c r="C10" t="s">
+        <v>122</v>
+      </c>
+      <c r="D10" s="9"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="10"/>
+      <c r="A11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" t="s">
+        <v>123</v>
+      </c>
+      <c r="C11" t="s">
+        <v>123</v>
+      </c>
+      <c r="D11" s="9"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>56</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="B12" t="s">
+        <v>124</v>
+      </c>
+      <c r="C12" t="s">
+        <v>124</v>
+      </c>
+      <c r="D12" s="9"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>58</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="B13" t="s">
+        <v>125</v>
+      </c>
+      <c r="C13" t="s">
+        <v>125</v>
+      </c>
+      <c r="D13" s="9"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="10"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="9"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="10"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="10"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="10"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="10"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D15" s="10"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="11" t="s">
+      <c r="B21" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D21" s="10"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="D16" s="10"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="11" t="s">
+      <c r="B22" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D22" s="10"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="D17" s="10"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="10"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="B19" t="s">
-        <v>79</v>
-      </c>
-      <c r="C19" t="s">
-        <v>79</v>
-      </c>
-      <c r="D19" s="10" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="B20" t="s">
-        <v>80</v>
-      </c>
-      <c r="C20" t="s">
-        <v>80</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="B21" t="s">
-        <v>81</v>
-      </c>
-      <c r="C21" t="s">
-        <v>81</v>
-      </c>
-      <c r="D21" s="10" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D22" s="10"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="B23" t="s">
-        <v>72</v>
-      </c>
-      <c r="C23" t="s">
-        <v>72</v>
+      <c r="B23" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="D23" s="10"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="B24" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="10"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" t="s">
         <v>73</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C25" t="s">
         <v>73</v>
       </c>
-      <c r="D24" s="10"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="B25" t="s">
+      <c r="D25" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B26" t="s">
+        <v>74</v>
+      </c>
+      <c r="C26" t="s">
+        <v>74</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B27" t="s">
+        <v>75</v>
+      </c>
+      <c r="C27" t="s">
+        <v>75</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D28" s="10"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B29" t="s">
+        <v>66</v>
+      </c>
+      <c r="C29" t="s">
+        <v>66</v>
+      </c>
+      <c r="D29" s="10"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B30" t="s">
+        <v>67</v>
+      </c>
+      <c r="C30" t="s">
+        <v>67</v>
+      </c>
+      <c r="D30" s="10"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B31" t="s">
         <v>21</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C31" t="s">
         <v>21</v>
       </c>
-      <c r="D25" s="10"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D26" s="10"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="B27" t="s">
-        <v>82</v>
-      </c>
-      <c r="C27" t="s">
-        <v>82</v>
-      </c>
-      <c r="E27" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="F27" s="10"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="B28" t="s">
-        <v>83</v>
-      </c>
-      <c r="C28" t="s">
-        <v>83</v>
-      </c>
-      <c r="E28" s="10" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="B29" t="s">
-        <v>84</v>
-      </c>
-      <c r="C29" t="s">
-        <v>84</v>
-      </c>
-      <c r="E29" s="10" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="B30" t="s">
-        <v>85</v>
-      </c>
-      <c r="C30" t="s">
-        <v>85</v>
-      </c>
-      <c r="E30" s="10" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="B31" t="s">
-        <v>86</v>
-      </c>
-      <c r="C31" t="s">
-        <v>86</v>
-      </c>
-      <c r="E31" s="10" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="B32" t="s">
-        <v>87</v>
-      </c>
-      <c r="C32" t="s">
-        <v>87</v>
-      </c>
-      <c r="E32" s="10" t="s">
-        <v>80</v>
-      </c>
+      <c r="D31" s="10"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D32" s="10"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B33" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="C33" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="E33" s="10" t="s">
-        <v>81</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="F33" s="10"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B34" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="C34" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="E34" s="10" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B35" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="C35" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="E35" s="10" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="11" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B36" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="C36" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="E36" s="10" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B37" t="s">
+        <v>80</v>
+      </c>
+      <c r="C37" t="s">
+        <v>80</v>
+      </c>
+      <c r="E37" s="10" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B38" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="B38" t="s">
+      <c r="C38" t="s">
+        <v>81</v>
+      </c>
+      <c r="E38" s="10" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B39" t="s">
         <v>82</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C39" t="s">
         <v>82</v>
       </c>
-      <c r="F38" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="B39" t="s">
-        <v>92</v>
-      </c>
-      <c r="C39" t="s">
-        <v>92</v>
-      </c>
-      <c r="F39" t="s">
+      <c r="E39" s="10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B40" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="B40" t="s">
-        <v>93</v>
-      </c>
       <c r="C40" t="s">
-        <v>93</v>
-      </c>
-      <c r="F40" t="s">
+        <v>83</v>
+      </c>
+      <c r="E40" s="10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B41" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="B41" t="s">
-        <v>94</v>
-      </c>
       <c r="C41" t="s">
-        <v>94</v>
-      </c>
-      <c r="F41" t="s">
+        <v>84</v>
+      </c>
+      <c r="E41" s="10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B42" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="B42" t="s">
-        <v>86</v>
-      </c>
       <c r="C42" t="s">
-        <v>86</v>
-      </c>
-      <c r="F42" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="B43" t="s">
-        <v>95</v>
-      </c>
-      <c r="C43" t="s">
-        <v>95</v>
-      </c>
-      <c r="F43" t="s">
-        <v>87</v>
+        <v>85</v>
+      </c>
+      <c r="E42" s="10" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="13" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B44" t="s">
-        <v>96</v>
+        <v>76</v>
       </c>
       <c r="C44" t="s">
-        <v>96</v>
+        <v>76</v>
       </c>
       <c r="F44" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="13" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B45" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="C45" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="F45" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="13" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B46" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="C46" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="F46" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="13" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B47" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="C47" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="F47" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="B48" t="s">
+        <v>80</v>
+      </c>
+      <c r="C48" t="s">
+        <v>80</v>
+      </c>
+      <c r="F48" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="B49" t="s">
+        <v>89</v>
+      </c>
+      <c r="C49" t="s">
+        <v>89</v>
+      </c>
+      <c r="F49" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="B50" t="s">
+        <v>90</v>
+      </c>
+      <c r="C50" t="s">
+        <v>90</v>
+      </c>
+      <c r="F50" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="B51" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="13"/>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="B49" t="s">
-        <v>100</v>
-      </c>
-      <c r="C49" s="16" t="s">
-        <v>100</v>
-      </c>
-      <c r="G49" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="B50" t="s">
-        <v>101</v>
-      </c>
-      <c r="C50" s="16" t="s">
-        <v>101</v>
-      </c>
-      <c r="G50" t="s">
+      <c r="C51" t="s">
+        <v>91</v>
+      </c>
+      <c r="F51" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="B52" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="B51" t="s">
-        <v>102</v>
-      </c>
-      <c r="C51" s="16" t="s">
-        <v>102</v>
-      </c>
-      <c r="G51" t="s">
+      <c r="C52" t="s">
+        <v>92</v>
+      </c>
+      <c r="F52" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="B53" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="B52" t="s">
-        <v>103</v>
-      </c>
-      <c r="C52" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="G52" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="B53" t="s">
-        <v>104</v>
-      </c>
-      <c r="C53" s="16" t="s">
-        <v>104</v>
-      </c>
-      <c r="G53" t="s">
-        <v>86</v>
+      <c r="C53" t="s">
+        <v>93</v>
+      </c>
+      <c r="F53" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="B54" t="s">
-        <v>105</v>
-      </c>
-      <c r="C54" s="16" t="s">
-        <v>105</v>
-      </c>
-      <c r="G54" t="s">
-        <v>95</v>
-      </c>
+      <c r="A54" s="13"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="11" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B55" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="C55" s="16" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="G55" t="s">
-        <v>96</v>
+        <v>76</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="11" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B56" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="C56" s="16" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="G56" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="11" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B57" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="C57" s="16" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="G57" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="11" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B58" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="C58" s="16" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="G58" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B59" t="s">
+        <v>98</v>
+      </c>
+      <c r="C59" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="G59" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B60" t="s">
         <v>99</v>
+      </c>
+      <c r="C60" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="G60" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>100</v>
+      </c>
+      <c r="C61" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="G61" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B62" t="s">
+        <v>101</v>
+      </c>
+      <c r="C62" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="G62" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B63" t="s">
+        <v>102</v>
+      </c>
+      <c r="C63" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="G63" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B64" t="s">
+        <v>103</v>
+      </c>
+      <c r="C64" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="G64" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-  <ignoredErrors>
-    <ignoredError sqref="C2:C5 B2:B5" numberStoredAsText="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
 
@@ -1953,21 +2039,21 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B2" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D2" t="s">
         <v>12</v>
@@ -1988,9 +2074,6 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="16384" width="9" style="17"/>
-  </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>